<commit_message>
PoPulando o Dashboard financeiro anual
</commit_message>
<xml_diff>
--- a/Projeto Final/projetoFluxodeCaixa.xlsx
+++ b/Projeto Final/projetoFluxodeCaixa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9825" windowHeight="7035" firstSheet="13" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9825" windowHeight="7035" firstSheet="14" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Início" sheetId="3" r:id="rId1"/>
@@ -52,7 +52,7 @@
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId20"/>
     <pivotCache cacheId="1" r:id="rId21"/>
-    <pivotCache cacheId="2" r:id="rId22"/>
+    <pivotCache cacheId="13" r:id="rId22"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{876F7934-8845-4945-9796-88D515C7AA90}">
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1775" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1772" uniqueCount="616">
   <si>
     <t>Vendas de mercadorias</t>
   </si>
@@ -1922,12 +1922,6 @@
     <t>Mês</t>
   </si>
   <si>
-    <t>Pagar Mensal</t>
-  </si>
-  <si>
-    <t>Receber Mensal</t>
-  </si>
-  <si>
     <t>Gráfico</t>
   </si>
   <si>
@@ -1980,6 +1974,17 @@
   </si>
   <si>
     <t>Resultado</t>
+  </si>
+  <si>
+    <t>Pagar 
+Mensal</t>
+  </si>
+  <si>
+    <t>Receber 
+Mensal</t>
+  </si>
+  <si>
+    <t>J F M A M J J A S O N D</t>
   </si>
 </sst>
 </file>
@@ -1994,7 +1999,7 @@
     <numFmt numFmtId="165" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
     <numFmt numFmtId="166" formatCode="&quot;R$&quot;\ #,##0"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2159,6 +2164,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -2222,7 +2243,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -2593,12 +2614,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFA6A6A6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFA6A6A6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFA6A6A6"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFA6A6A6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFA6A6A6"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFA6A6A6"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFA6A6A6"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFA6A6A6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFA6A6A6"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFA6A6A6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2759,18 +2842,6 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2780,12 +2851,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2843,12 +2908,6 @@
     <xf numFmtId="43" fontId="17" fillId="9" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="15" fillId="9" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -2891,6 +2950,33 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2906,38 +2992,104 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="14" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="15" fillId="9" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="15" fillId="9" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="15" fillId="9" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="15" fillId="9" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="15" fillId="9" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="15" fillId="9" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="22" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="22" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="46">
     <dxf>
       <font>
         <b/>
         <i val="0"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFC00000"/>
       </font>
     </dxf>
     <dxf>
@@ -3154,6 +3306,818 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Dashboard financeiro anualD'!$M$6:$M$17</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Jan</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Fev</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Mar</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mai</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Jun</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Jul</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Ago</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Set</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Out</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Nov</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Dez</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Dashboard financeiro anualD'!$L$6:$L$17</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2564</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4732</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5489</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>618</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1654</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>555</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1406347648"/>
+        <c:axId val="1406350912"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1406347648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1406350912"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1406350912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1406347648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6337,6 +7301,38 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>219076</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>323850</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8676,7 +9672,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Autor" refreshedDate="45386.700453472222" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="231">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Autor" refreshedDate="45392.752931134259" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="231">
   <cacheSource type="worksheet">
     <worksheetSource name="TbRegistroEntradas" r:id="rId2"/>
   </cacheSource>
@@ -15975,7 +16971,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TDDetalhamentoReceita" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TDDetalhamentoReceita" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B5:O13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -16108,13 +17104,13 @@
     <dataField name="Soma de Valor" fld="6" baseField="4" baseItem="2" numFmtId="4"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="8">
+    <format dxfId="11">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="7">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="6">
+    <format dxfId="9">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -16293,7 +17289,7 @@
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TDContasAPagar" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B6:L14" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <location ref="B6:G12" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="13">
     <pivotField showAll="0"/>
     <pivotField numFmtId="14" showAll="0"/>
@@ -16367,15 +17363,9 @@
     <field x="3"/>
     <field x="4"/>
   </rowFields>
-  <rowItems count="6">
+  <rowItems count="4">
     <i>
       <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
     </i>
     <i r="1">
       <x v="3"/>
@@ -16391,19 +17381,13 @@
     <field x="7"/>
     <field x="11"/>
   </colFields>
-  <colItems count="10">
+  <colItems count="5">
     <i>
       <x/>
       <x/>
     </i>
     <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
       <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="5"/>
     </i>
     <i r="1">
       <x v="6"/>
@@ -16411,40 +17395,31 @@
     <i r="1">
       <x v="7"/>
     </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
-    <i r="1">
-      <x v="9"/>
-    </i>
-    <i r="1">
-      <x v="11"/>
-    </i>
     <i t="default">
       <x/>
     </i>
   </colItems>
   <pageFields count="1">
-    <pageField fld="12" hier="-1"/>
+    <pageField fld="12" item="2" hier="-1"/>
   </pageFields>
   <dataFields count="1">
     <dataField name="Soma de Valor" fld="6" baseField="3" baseItem="0" numFmtId="4"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="5">
+    <format dxfId="8">
       <pivotArea field="12" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="4">
+    <format dxfId="7">
       <pivotArea field="12" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="3">
+    <format dxfId="6">
       <pivotArea dataOnly="0" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="12" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="5">
       <pivotArea dataOnly="0" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="12" count="0"/>
@@ -16462,8 +17437,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TDContasAReceber" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="B5:M13" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TDContasAReceber" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="B5:G12" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
     <pivotField numFmtId="14" showAll="0"/>
@@ -16536,15 +17511,12 @@
     <field x="3"/>
     <field x="4"/>
   </rowFields>
-  <rowItems count="6">
+  <rowItems count="5">
     <i>
       <x/>
     </i>
     <i r="1">
       <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
     </i>
     <i r="1">
       <x v="3"/>
@@ -16560,7 +17532,7 @@
     <field x="7"/>
     <field x="11"/>
   </colFields>
-  <colItems count="11">
+  <colItems count="5">
     <i>
       <x/>
       <x/>
@@ -16572,32 +17544,14 @@
       <x v="4"/>
     </i>
     <i r="1">
-      <x v="5"/>
-    </i>
-    <i r="1">
       <x v="6"/>
-    </i>
-    <i r="1">
-      <x v="7"/>
-    </i>
-    <i r="1">
-      <x v="8"/>
-    </i>
-    <i r="1">
-      <x v="9"/>
-    </i>
-    <i r="1">
-      <x v="10"/>
-    </i>
-    <i r="1">
-      <x v="11"/>
     </i>
     <i t="default">
       <x/>
     </i>
   </colItems>
   <pageFields count="1">
-    <pageField fld="12" hier="-1"/>
+    <pageField fld="12" item="2" hier="-1"/>
   </pageFields>
   <dataFields count="1">
     <dataField name="Soma de Valor" fld="6" baseField="3" baseItem="0" numFmtId="4"/>
@@ -16612,7 +17566,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TDContasAReceberVencidas" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TDContasAReceberVencidas" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B6:L14" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -16871,17 +17825,17 @@
     <tabular pivotCacheId="3">
       <items count="12">
         <i x="4" s="1"/>
-        <i x="6" s="1"/>
         <i x="7" s="1"/>
-        <i x="9" s="1"/>
         <i x="10" s="1"/>
         <i x="11" s="1"/>
-        <i x="1" s="1"/>
-        <i x="0" s="1"/>
-        <i x="3" s="1"/>
         <i x="5" s="1" nd="1"/>
+        <i x="6" s="1" nd="1"/>
         <i x="8" s="1" nd="1"/>
+        <i x="9" s="1" nd="1"/>
+        <i x="1" s="1" nd="1"/>
+        <i x="0" s="1" nd="1"/>
         <i x="2" s="1" nd="1"/>
+        <i x="3" s="1" nd="1"/>
       </items>
     </tabular>
   </data>
@@ -16896,8 +17850,8 @@
   <data>
     <tabular pivotCacheId="3">
       <items count="3">
-        <i x="0" s="1"/>
-        <i x="1" s="1"/>
+        <i x="0"/>
+        <i x="1"/>
         <i x="2" s="1"/>
       </items>
     </tabular>
@@ -16916,15 +17870,15 @@
         <i x="5" s="1"/>
         <i x="8" s="1"/>
         <i x="9" s="1"/>
-        <i x="10" s="1"/>
         <i x="11" s="1"/>
-        <i x="0" s="1"/>
-        <i x="1" s="1"/>
-        <i x="2" s="1"/>
-        <i x="3" s="1"/>
-        <i x="4" s="1"/>
         <i x="6" s="1" nd="1"/>
         <i x="7" s="1" nd="1"/>
+        <i x="10" s="1" nd="1"/>
+        <i x="0" s="1" nd="1"/>
+        <i x="1" s="1" nd="1"/>
+        <i x="2" s="1" nd="1"/>
+        <i x="3" s="1" nd="1"/>
+        <i x="4" s="1" nd="1"/>
       </items>
     </tabular>
   </data>
@@ -16944,8 +17898,8 @@
   <data>
     <tabular pivotCacheId="1">
       <items count="3">
-        <i x="0" s="1"/>
-        <i x="1" s="1"/>
+        <i x="0"/>
+        <i x="1"/>
         <i x="2" s="1"/>
       </items>
     </tabular>
@@ -16994,7 +17948,7 @@
 <file path=xl/slicers/slicer4.xml><?xml version="1.0" encoding="utf-8"?>
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
   <slicer name="Mês previsto 1" cache="SegmentaçãodeDados_Mês_previsto1" caption="Mês previsto" columnCount="6" rowHeight="241300"/>
-  <slicer name="Ano Previsto 1" cache="SegmentaçãodeDados_Ano_Previsto1" caption="Ano Previsto" rowHeight="241300"/>
+  <slicer name="Ano Previsto 1" cache="SegmentaçãodeDados_Ano_Previsto1" caption="Ano Previsto" startItem="2" rowHeight="241300"/>
 </slicers>
 </file>
 
@@ -17005,7 +17959,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbPCEntradasN1" displayName="TbPCEntradasN1" ref="B4:B10" totalsRowShown="0" headerRowDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TbPCEntradasN1" displayName="TbPCEntradasN1" ref="B4:B10" totalsRowShown="0" headerRowDxfId="45">
   <autoFilter ref="B4:B10"/>
   <tableColumns count="1">
     <tableColumn id="1" name="Nível 1"/>
@@ -17047,7 +18001,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TbRegistroEntradas" displayName="TbRegistroEntradas" ref="B5:O236" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="TbRegistroEntradas" displayName="TbRegistroEntradas" ref="B5:O236" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
   <autoFilter ref="B5:O236">
     <filterColumn colId="8">
       <filters>
@@ -17056,39 +18010,39 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="14">
-    <tableColumn id="1" name="Data do Caixa Realizado" dataDxfId="39"/>
-    <tableColumn id="2" name="Data da Competência" dataDxfId="38"/>
-    <tableColumn id="3" name="Data do Caixa Previsto" dataDxfId="37"/>
-    <tableColumn id="4" name="Conta Nível 1" dataDxfId="36"/>
-    <tableColumn id="5" name="Conta Nível 2" dataDxfId="35"/>
-    <tableColumn id="6" name="Histórico" dataDxfId="34"/>
-    <tableColumn id="7" name="Valor" dataDxfId="33"/>
-    <tableColumn id="8" name="Mês Caixa" dataDxfId="32">
+    <tableColumn id="1" name="Data do Caixa Realizado" dataDxfId="42"/>
+    <tableColumn id="2" name="Data da Competência" dataDxfId="41"/>
+    <tableColumn id="3" name="Data do Caixa Previsto" dataDxfId="40"/>
+    <tableColumn id="4" name="Conta Nível 1" dataDxfId="39"/>
+    <tableColumn id="5" name="Conta Nível 2" dataDxfId="38"/>
+    <tableColumn id="6" name="Histórico" dataDxfId="37"/>
+    <tableColumn id="7" name="Valor" dataDxfId="36"/>
+    <tableColumn id="8" name="Mês Caixa" dataDxfId="35">
       <calculatedColumnFormula>IF(TbRegistroEntradas[[#This Row],[Data do Caixa Realizado]]="",0,MONTH(TbRegistroEntradas[[#This Row],[Data do Caixa Realizado]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Ano Caixa" dataDxfId="31">
+    <tableColumn id="9" name="Ano Caixa" dataDxfId="34">
       <calculatedColumnFormula>IF(TbRegistroEntradas[[#This Row],[Data do Caixa Realizado]]="",0,YEAR(TbRegistroEntradas[[#This Row],[Data do Caixa Realizado]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Mês _x000a_Competência" dataDxfId="30">
+    <tableColumn id="10" name="Mês _x000a_Competência" dataDxfId="33">
       <calculatedColumnFormula>IF(TbRegistroEntradas[[#This Row],[Data da Competência]]="",0,MONTH(TbRegistroEntradas[[#This Row],[Data da Competência]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Ano _x000a_Competência" dataDxfId="29">
+    <tableColumn id="11" name="Ano _x000a_Competência" dataDxfId="32">
       <calculatedColumnFormula>IF(TbRegistroEntradas[[#This Row],[Data da Competência]]="",0,YEAR(TbRegistroEntradas[[#This Row],[Data da Competência]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Mês previsto" dataDxfId="28">
+    <tableColumn id="12" name="Mês previsto" dataDxfId="31">
       <calculatedColumnFormula>IF(TbRegistroEntradas[[#This Row],[Data do Caixa Previsto]]="",0,MONTH(TbRegistroEntradas[[#This Row],[Data do Caixa Previsto]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Ano Previsto" dataDxfId="27">
+    <tableColumn id="13" name="Ano Previsto" dataDxfId="30">
       <calculatedColumnFormula>IF(TbRegistroEntradas[[#This Row],[Data do Caixa Previsto]]="",0,YEAR(TbRegistroEntradas[[#This Row],[Data do Caixa Previsto]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Conta vencida" dataDxfId="26"/>
+    <tableColumn id="14" name="Conta vencida" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="TbRegistrosSaida" displayName="TbRegistrosSaida" ref="B5:N234" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="TbRegistrosSaida" displayName="TbRegistrosSaida" ref="B5:N234" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25">
   <autoFilter ref="B5:N234">
     <filterColumn colId="8">
       <filters>
@@ -17097,29 +18051,29 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" name="Data do Caixa Realizado" dataDxfId="21"/>
-    <tableColumn id="2" name="Data da Competência" dataDxfId="20"/>
-    <tableColumn id="3" name="Data do Caixa Previsto" dataDxfId="19"/>
-    <tableColumn id="4" name="Conta Nível 1" dataDxfId="18"/>
-    <tableColumn id="5" name="Conta Nível 2" dataDxfId="17"/>
-    <tableColumn id="6" name="Histórico" dataDxfId="16"/>
-    <tableColumn id="7" name="Valor" dataDxfId="15"/>
-    <tableColumn id="8" name="Mês Caixa" dataDxfId="14">
+    <tableColumn id="1" name="Data do Caixa Realizado" dataDxfId="24"/>
+    <tableColumn id="2" name="Data da Competência" dataDxfId="23"/>
+    <tableColumn id="3" name="Data do Caixa Previsto" dataDxfId="22"/>
+    <tableColumn id="4" name="Conta Nível 1" dataDxfId="21"/>
+    <tableColumn id="5" name="Conta Nível 2" dataDxfId="20"/>
+    <tableColumn id="6" name="Histórico" dataDxfId="19"/>
+    <tableColumn id="7" name="Valor" dataDxfId="18"/>
+    <tableColumn id="8" name="Mês Caixa" dataDxfId="17">
       <calculatedColumnFormula>IF(TbRegistrosSaida[[#This Row],[Data do Caixa Realizado]]="",0,MONTH(TbRegistrosSaida[[#This Row],[Data do Caixa Realizado]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Ano Caixa" dataDxfId="13">
+    <tableColumn id="9" name="Ano Caixa" dataDxfId="16">
       <calculatedColumnFormula>IF(TbRegistrosSaida[[#This Row],[Data do Caixa Realizado]]="",0,YEAR(TbRegistrosSaida[[#This Row],[Data do Caixa Realizado]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Mês _x000a_Competência" dataDxfId="12">
+    <tableColumn id="10" name="Mês _x000a_Competência" dataDxfId="15">
       <calculatedColumnFormula>IF(TbRegistrosSaida[[#This Row],[Data da Competência]]="",0,MONTH(TbRegistrosSaida[[#This Row],[Data da Competência]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Ano _x000a_Competência" dataDxfId="11">
+    <tableColumn id="11" name="Ano _x000a_Competência" dataDxfId="14">
       <calculatedColumnFormula>IF(TbRegistrosSaida[[#This Row],[Data da Competência]]="",0,YEAR(TbRegistrosSaida[[#This Row],[Data da Competência]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Mês previsto" dataDxfId="10">
+    <tableColumn id="12" name="Mês previsto" dataDxfId="13">
       <calculatedColumnFormula>IF(TbRegistrosSaida[[#This Row],[Data do Caixa Previsto]]="",0,MONTH(TbRegistrosSaida[[#This Row],[Data do Caixa Previsto]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="Ano Previsto" dataDxfId="9">
+    <tableColumn id="13" name="Ano Previsto" dataDxfId="12">
       <calculatedColumnFormula>IF(TbRegistrosSaida[[#This Row],[Data do Caixa Previsto]]="",0,YEAR(TbRegistrosSaida[[#This Row],[Data do Caixa Previsto]]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -17416,7 +18370,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="H1" workbookViewId="0"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18377,7 +19333,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18428,8 +19384,8 @@
       <c r="B4" s="60" t="s">
         <v>573</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>565</v>
+      <c r="C4" s="22">
+        <v>2019</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18445,7 +19401,7 @@
       <c r="C7">
         <v>0</v>
       </c>
-      <c r="L7" t="s">
+      <c r="G7" t="s">
         <v>574</v>
       </c>
     </row>
@@ -18457,28 +19413,13 @@
         <v>1</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E8">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F8">
-        <v>6</v>
-      </c>
-      <c r="G8">
-        <v>7</v>
-      </c>
-      <c r="H8">
         <v>8</v>
-      </c>
-      <c r="I8">
-        <v>9</v>
-      </c>
-      <c r="J8">
-        <v>10</v>
-      </c>
-      <c r="K8">
-        <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -18486,159 +19427,75 @@
         <v>16</v>
       </c>
       <c r="C9" s="61">
-        <v>6314</v>
+        <v>5159</v>
       </c>
       <c r="D9" s="61">
-        <v>4438</v>
+        <v>1753</v>
       </c>
       <c r="E9" s="61">
-        <v>1753</v>
+        <v>2338</v>
       </c>
       <c r="F9" s="61">
-        <v>701</v>
+        <v>2759</v>
       </c>
       <c r="G9" s="61">
-        <v>2338</v>
-      </c>
-      <c r="H9" s="61">
-        <v>6976</v>
-      </c>
-      <c r="I9" s="61">
-        <v>1565</v>
-      </c>
-      <c r="J9" s="61">
-        <v>5873</v>
-      </c>
-      <c r="K9" s="61">
-        <v>1967</v>
-      </c>
-      <c r="L9" s="61">
-        <v>31925</v>
+        <v>12009</v>
       </c>
     </row>
     <row r="10" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="55" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
+      <c r="D10" s="61">
+        <v>1753</v>
+      </c>
       <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61">
-        <v>4217</v>
-      </c>
-      <c r="I10" s="61">
-        <v>1565</v>
-      </c>
-      <c r="J10" s="61"/>
-      <c r="K10" s="61"/>
-      <c r="L10" s="61">
-        <v>5782</v>
+      <c r="F10" s="61">
+        <v>2759</v>
+      </c>
+      <c r="G10" s="61">
+        <v>4512</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="55" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="61"/>
+        <v>78</v>
+      </c>
+      <c r="C11" s="61">
+        <v>5159</v>
+      </c>
       <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
+      <c r="E11" s="61">
+        <v>2338</v>
+      </c>
       <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="61">
-        <v>5873</v>
-      </c>
-      <c r="K11" s="61"/>
-      <c r="L11" s="61">
-        <v>5873</v>
+      <c r="G11" s="61">
+        <v>7497</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
+      <c r="B12" s="54" t="s">
+        <v>567</v>
+      </c>
+      <c r="C12" s="61">
+        <v>5159</v>
+      </c>
+      <c r="D12" s="61">
+        <v>1753</v>
+      </c>
       <c r="E12" s="61">
-        <v>1753</v>
-      </c>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="61">
+        <v>2338</v>
+      </c>
+      <c r="F12" s="61">
         <v>2759</v>
       </c>
-      <c r="I12" s="61"/>
-      <c r="J12" s="61"/>
-      <c r="K12" s="61"/>
-      <c r="L12" s="61">
-        <v>4512</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="55" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="61">
-        <v>6314</v>
-      </c>
-      <c r="D13" s="61">
-        <v>4438</v>
-      </c>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61">
-        <v>701</v>
-      </c>
-      <c r="G13" s="61">
-        <v>2338</v>
-      </c>
-      <c r="H13" s="61"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="61"/>
-      <c r="K13" s="61">
-        <v>1967</v>
-      </c>
-      <c r="L13" s="61">
-        <v>15758</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="54" t="s">
-        <v>567</v>
-      </c>
-      <c r="C14" s="61">
-        <v>6314</v>
-      </c>
-      <c r="D14" s="61">
-        <v>4438</v>
-      </c>
-      <c r="E14" s="61">
-        <v>1753</v>
-      </c>
-      <c r="F14" s="61">
-        <v>701</v>
-      </c>
-      <c r="G14" s="61">
-        <v>2338</v>
-      </c>
-      <c r="H14" s="61">
-        <v>6976</v>
-      </c>
-      <c r="I14" s="61">
-        <v>1565</v>
-      </c>
-      <c r="J14" s="61">
-        <v>5873</v>
-      </c>
-      <c r="K14" s="61">
-        <v>1967</v>
-      </c>
-      <c r="L14" s="61">
-        <v>31925</v>
-      </c>
-    </row>
+      <c r="G12" s="61">
+        <v>12009</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18662,8 +19519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18713,8 +19570,8 @@
       <c r="B3" s="53" t="s">
         <v>573</v>
       </c>
-      <c r="C3" t="s">
-        <v>565</v>
+      <c r="C3" s="54">
+        <v>2019</v>
       </c>
     </row>
     <row r="4" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18730,7 +19587,7 @@
       <c r="C6">
         <v>0</v>
       </c>
-      <c r="M6" t="s">
+      <c r="G6" t="s">
         <v>574</v>
       </c>
     </row>
@@ -18748,25 +19605,7 @@
         <v>5</v>
       </c>
       <c r="F7">
-        <v>6</v>
-      </c>
-      <c r="G7">
         <v>7</v>
-      </c>
-      <c r="H7">
-        <v>8</v>
-      </c>
-      <c r="I7">
-        <v>9</v>
-      </c>
-      <c r="J7">
-        <v>10</v>
-      </c>
-      <c r="K7">
-        <v>11</v>
-      </c>
-      <c r="L7">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -18774,185 +19613,90 @@
         <v>0</v>
       </c>
       <c r="C8" s="57">
-        <v>1767</v>
+        <v>483</v>
       </c>
       <c r="D8" s="57">
-        <v>3316</v>
+        <v>928</v>
       </c>
       <c r="E8" s="57">
         <v>2015</v>
       </c>
       <c r="F8" s="57">
-        <v>6102</v>
+        <v>1987</v>
       </c>
       <c r="G8" s="57">
-        <v>1987</v>
-      </c>
-      <c r="H8" s="57">
-        <v>770</v>
-      </c>
-      <c r="I8" s="57">
-        <v>4253</v>
-      </c>
-      <c r="J8" s="57">
-        <v>9905</v>
-      </c>
-      <c r="K8" s="57">
-        <v>1171</v>
-      </c>
-      <c r="L8" s="57">
-        <v>6972</v>
-      </c>
-      <c r="M8" s="57">
-        <v>38258</v>
+        <v>5413</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="57">
-        <v>1284</v>
-      </c>
+      <c r="C9" s="57"/>
       <c r="D9" s="57"/>
       <c r="E9" s="57"/>
       <c r="F9" s="57">
-        <v>3878</v>
+        <v>508</v>
       </c>
       <c r="G9" s="57">
         <v>508</v>
       </c>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="57">
-        <v>4922</v>
-      </c>
-      <c r="K9" s="57"/>
-      <c r="L9" s="57">
-        <v>919</v>
-      </c>
-      <c r="M9" s="57">
-        <v>11511</v>
-      </c>
     </row>
     <row r="10" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="55" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C10" s="57"/>
       <c r="D10" s="57">
-        <v>2388</v>
-      </c>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="57">
-        <v>1171</v>
-      </c>
-      <c r="L10" s="57"/>
-      <c r="M10" s="57">
-        <v>3559</v>
+        <v>928</v>
+      </c>
+      <c r="E10" s="57">
+        <v>667</v>
+      </c>
+      <c r="F10" s="57">
+        <v>1479</v>
+      </c>
+      <c r="G10" s="57">
+        <v>3074</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57">
-        <v>928</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C11" s="57">
+        <v>483</v>
+      </c>
+      <c r="D11" s="57"/>
       <c r="E11" s="57">
-        <v>667</v>
-      </c>
-      <c r="F11" s="57">
-        <v>2224</v>
-      </c>
+        <v>1348</v>
+      </c>
+      <c r="F11" s="57"/>
       <c r="G11" s="57">
-        <v>1479</v>
-      </c>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57">
-        <v>4253</v>
-      </c>
-      <c r="J11" s="57">
-        <v>4983</v>
-      </c>
-      <c r="K11" s="57"/>
-      <c r="L11" s="57">
-        <v>1414</v>
-      </c>
-      <c r="M11" s="57">
-        <v>15948</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="55" t="s">
-        <v>50</v>
+      <c r="B12" s="54" t="s">
+        <v>567</v>
       </c>
       <c r="C12" s="57">
         <v>483</v>
       </c>
-      <c r="D12" s="57"/>
+      <c r="D12" s="57">
+        <v>928</v>
+      </c>
       <c r="E12" s="57">
-        <v>1348</v>
-      </c>
-      <c r="F12" s="57"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57">
-        <v>770</v>
-      </c>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="57">
-        <v>4639</v>
-      </c>
-      <c r="M12" s="57">
-        <v>7240</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="54" t="s">
-        <v>567</v>
-      </c>
-      <c r="C13" s="57">
-        <v>1767</v>
-      </c>
-      <c r="D13" s="57">
-        <v>3316</v>
-      </c>
-      <c r="E13" s="57">
         <v>2015</v>
       </c>
-      <c r="F13" s="57">
-        <v>6102</v>
-      </c>
-      <c r="G13" s="57">
+      <c r="F12" s="57">
         <v>1987</v>
       </c>
-      <c r="H13" s="57">
-        <v>770</v>
-      </c>
-      <c r="I13" s="57">
-        <v>4253</v>
-      </c>
-      <c r="J13" s="57">
-        <v>9905</v>
-      </c>
-      <c r="K13" s="57">
-        <v>1171</v>
-      </c>
-      <c r="L13" s="57">
-        <v>6972</v>
-      </c>
-      <c r="M13" s="57">
-        <v>38258</v>
-      </c>
-    </row>
+      <c r="G12" s="57">
+        <v>5413</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19018,12 +19762,12 @@
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
-      <c r="N2" s="69">
+      <c r="N2" s="114">
         <f ca="1">TODAY()</f>
-        <v>45390</v>
-      </c>
-      <c r="O2" s="69"/>
-      <c r="P2" s="69"/>
+        <v>45392</v>
+      </c>
+      <c r="O2" s="114"/>
+      <c r="P2" s="114"/>
     </row>
     <row r="3" spans="2:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -19276,8 +20020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19286,12 +20030,13 @@
     <col min="2" max="2" width="39.7109375" customWidth="1"/>
     <col min="3" max="3" width="1.42578125" customWidth="1"/>
     <col min="4" max="4" width="39.7109375" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" customWidth="1"/>
+    <col min="5" max="5" width="2.5703125" customWidth="1"/>
     <col min="6" max="7" width="16.28515625" customWidth="1"/>
     <col min="8" max="8" width="1.7109375" customWidth="1"/>
     <col min="9" max="10" width="16.28515625" customWidth="1"/>
-    <col min="11" max="11" width="1.7109375" customWidth="1"/>
-    <col min="12" max="13" width="16.28515625" customWidth="1"/>
+    <col min="11" max="11" width="4.5703125" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
     <col min="14" max="14" width="10" customWidth="1"/>
     <col min="15" max="15" width="9.140625" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" hidden="1"/>
@@ -19324,222 +20069,314 @@
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70">
+      <c r="L2" s="62"/>
+      <c r="M2" s="62">
         <v>2019</v>
       </c>
     </row>
     <row r="3" spans="2:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="113" t="s">
+      <c r="B4" s="101" t="s">
         <v>577</v>
       </c>
-      <c r="D4" s="113" t="s">
+      <c r="D4" s="101" t="s">
         <v>578</v>
       </c>
-      <c r="F4" s="114" t="s">
+      <c r="F4" s="115" t="s">
         <v>580</v>
       </c>
-      <c r="G4" s="115"/>
-      <c r="H4" s="115"/>
-      <c r="I4" s="115"/>
-      <c r="J4" s="115"/>
-      <c r="K4" s="115"/>
-      <c r="L4" s="115"/>
-      <c r="M4" s="116"/>
+      <c r="G4" s="116"/>
+      <c r="H4" s="116"/>
+      <c r="I4" s="116"/>
+      <c r="J4" s="116"/>
+      <c r="K4" s="102"/>
+      <c r="L4" s="138" t="s">
+        <v>50</v>
+      </c>
+      <c r="M4" s="139"/>
     </row>
     <row r="5" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="119">
+      <c r="B5" s="140">
         <f>'Dashboard financeiro anualD'!D12</f>
         <v>-3097</v>
       </c>
-      <c r="D5" s="119"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="73"/>
+      <c r="D5" s="134" t="s">
+        <v>615</v>
+      </c>
+      <c r="F5" s="63"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="65"/>
     </row>
     <row r="6" spans="2:13" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F6" s="71"/>
-      <c r="G6" s="72"/>
-      <c r="H6" s="72"/>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="73"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="65"/>
     </row>
     <row r="7" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="113" t="s">
+      <c r="B7" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="113"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="72"/>
-      <c r="H7" s="72"/>
-      <c r="I7" s="72"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="72"/>
-      <c r="L7" s="125" t="s">
+      <c r="D7" s="132"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="64"/>
+      <c r="L7" s="135" t="s">
         <v>581</v>
       </c>
-      <c r="M7" s="73"/>
+      <c r="M7" s="136"/>
     </row>
     <row r="8" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="119">
+      <c r="B8" s="140">
+        <f>'Dashboard financeiro anualD'!E14</f>
+        <v>12009</v>
+      </c>
+      <c r="D8" s="133"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="103">
         <v>9999</v>
       </c>
-      <c r="D8" s="119"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="120">
-        <v>9999</v>
-      </c>
-      <c r="L8" s="120"/>
-      <c r="M8" s="121"/>
+      <c r="L8" s="137">
+        <f>SUM('Dashboard financeiro anualD'!K6:K17)</f>
+        <v>15612</v>
+      </c>
+      <c r="M8" s="122"/>
     </row>
     <row r="9" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F9" s="71"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
-      <c r="I9" s="72"/>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="72"/>
-      <c r="M9" s="73"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="64"/>
+      <c r="J9" s="64"/>
+      <c r="K9" s="64"/>
+      <c r="L9" s="64"/>
+      <c r="M9" s="65"/>
     </row>
     <row r="10" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="113" t="s">
+      <c r="B10" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="113"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="72"/>
-      <c r="H10" s="72"/>
-      <c r="I10" s="72"/>
-      <c r="J10" s="72"/>
-      <c r="K10" s="72"/>
-      <c r="L10" s="72"/>
-      <c r="M10" s="73"/>
-    </row>
-    <row r="11" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="119">
-        <v>9999</v>
-      </c>
-      <c r="D11" s="119"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
-      <c r="I11" s="75"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="75"/>
-      <c r="L11" s="75"/>
-      <c r="M11" s="76"/>
+      <c r="D10" s="132"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="64"/>
+      <c r="J10" s="64"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="64"/>
+      <c r="M10" s="65"/>
+    </row>
+    <row r="11" spans="2:13" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="140">
+        <f>'Dashboard financeiro anualD'!E15</f>
+        <v>5413</v>
+      </c>
+      <c r="D11" s="133"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="67"/>
+      <c r="L11" s="67"/>
+      <c r="M11" s="68"/>
     </row>
     <row r="12" spans="2:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="114" t="s">
+      <c r="B13" s="115" t="s">
         <v>579</v>
       </c>
-      <c r="C13" s="115"/>
-      <c r="D13" s="116"/>
-      <c r="F13" s="117" t="s">
+      <c r="C13" s="116"/>
+      <c r="D13" s="117"/>
+      <c r="F13" s="118" t="s">
         <v>582</v>
       </c>
-      <c r="G13" s="118"/>
-      <c r="I13" s="117" t="s">
+      <c r="G13" s="119"/>
+      <c r="I13" s="118" t="s">
         <v>586</v>
       </c>
-      <c r="J13" s="118"/>
-      <c r="L13" s="117" t="s">
+      <c r="J13" s="119"/>
+      <c r="L13" s="118" t="s">
         <v>587</v>
       </c>
-      <c r="M13" s="118"/>
+      <c r="M13" s="119"/>
     </row>
     <row r="14" spans="2:13" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="71"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="73"/>
-      <c r="F14" s="71"/>
-      <c r="G14" s="73"/>
-      <c r="I14" s="71"/>
-      <c r="J14" s="73"/>
-      <c r="L14" s="71"/>
-      <c r="M14" s="73"/>
-    </row>
-    <row r="15" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="119">
+      <c r="B14" s="63"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="65"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="65"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="65"/>
+      <c r="L14" s="63"/>
+      <c r="M14" s="65"/>
+    </row>
+    <row r="15" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="141">
         <v>9999</v>
       </c>
-      <c r="C15" s="72"/>
-      <c r="D15" s="73"/>
-      <c r="F15" s="77" t="s">
+      <c r="C15" s="64"/>
+      <c r="D15" s="65"/>
+      <c r="F15" s="69" t="s">
         <v>583</v>
       </c>
-      <c r="G15" s="78" t="s">
+      <c r="G15" s="70" t="s">
         <v>584</v>
       </c>
-      <c r="I15" s="79"/>
-      <c r="J15" s="80"/>
-      <c r="L15" s="71"/>
-      <c r="M15" s="73"/>
+      <c r="I15" s="120"/>
+      <c r="J15" s="121"/>
+      <c r="L15" s="63"/>
+      <c r="M15" s="65"/>
     </row>
     <row r="16" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="71"/>
-      <c r="C16" s="72"/>
-      <c r="D16" s="73"/>
-      <c r="F16" s="71"/>
-      <c r="G16" s="73"/>
-      <c r="I16" s="71"/>
-      <c r="J16" s="73"/>
-      <c r="L16" s="71"/>
-      <c r="M16" s="73"/>
+      <c r="B16" s="63"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="65"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="65"/>
+      <c r="I16" s="63"/>
+      <c r="J16" s="65"/>
+      <c r="L16" s="63"/>
+      <c r="M16" s="65"/>
     </row>
     <row r="17" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="71"/>
-      <c r="C17" s="72"/>
-      <c r="D17" s="73"/>
-      <c r="F17" s="122" t="s">
+      <c r="B17" s="63"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="65"/>
+      <c r="F17" s="104" t="s">
         <v>585</v>
       </c>
-      <c r="G17" s="123" t="s">
+      <c r="G17" s="105" t="s">
         <v>585</v>
       </c>
-      <c r="I17" s="71"/>
-      <c r="J17" s="73"/>
-      <c r="L17" s="71"/>
-      <c r="M17" s="73"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="65"/>
+      <c r="L17" s="63"/>
+      <c r="M17" s="65"/>
     </row>
     <row r="18" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="74"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="76"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="76"/>
-      <c r="I18" s="74"/>
-      <c r="J18" s="76"/>
-      <c r="L18" s="74"/>
-      <c r="M18" s="76"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="68"/>
+      <c r="F18" s="66"/>
+      <c r="G18" s="68"/>
+      <c r="I18" s="66"/>
+      <c r="J18" s="68"/>
+      <c r="L18" s="66"/>
+      <c r="M18" s="68"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="11">
+    <mergeCell ref="L13:M13"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="F4:J4"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="L8:M8"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K8:M8"/>
-    <mergeCell ref="F4:M4"/>
-    <mergeCell ref="L13:M13"/>
   </mergeCells>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4:M4">
+      <formula1>pcEntradasN2N2</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
+      <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap">
+          <x14:colorSeries rgb="FF00B050"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Dashboard financeiro anualD'!I6:I17</xm:f>
+              <xm:sqref>D10</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap">
+          <x14:colorSeries rgb="FFFF0000"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Dashboard financeiro anualD'!H6:H17</xm:f>
+              <xm:sqref>D7</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup type="column" displayEmptyCellsAs="gap">
+          <x14:colorSeries rgb="FF00B050"/>
+          <x14:colorNegative rgb="FFD00000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FFD00000"/>
+          <x14:colorFirst rgb="FFD00000"/>
+          <x14:colorLast rgb="FFD00000"/>
+          <x14:colorHigh rgb="FFD00000"/>
+          <x14:colorLow rgb="FFD00000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Dashboard financeiro anualD'!H6:H17</xm:f>
+              <xm:sqref>D11</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+      </x14:sparklineGroups>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -19547,792 +20384,980 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView showGridLines="0" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="81"/>
-      <c r="C2" s="82" t="s">
+      <c r="B2" s="71"/>
+      <c r="C2" s="72" t="s">
         <v>589</v>
       </c>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
-      <c r="L2" s="82"/>
-      <c r="M2" s="82"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="81"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="71"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="81"/>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="83" t="s">
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="73" t="s">
         <v>590</v>
       </c>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="83" t="s">
+      <c r="H4" s="71"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="73" t="s">
         <v>591</v>
       </c>
-      <c r="L4" s="84" t="s">
+      <c r="L4" s="74" t="s">
         <v>592</v>
       </c>
-      <c r="M4" s="85"/>
+      <c r="M4" s="75">
+        <f>D5</f>
+        <v>2019</v>
+      </c>
     </row>
     <row r="5" spans="2:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="81"/>
-      <c r="C5" s="84" t="s">
+      <c r="B5" s="71"/>
+      <c r="C5" s="74" t="s">
         <v>593</v>
       </c>
-      <c r="D5" s="86">
+      <c r="D5" s="76">
         <f>'Dashboard financeiro anual'!M2</f>
         <v>2019</v>
       </c>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="87" t="s">
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="77" t="s">
         <v>594</v>
       </c>
-      <c r="H5" s="88" t="s">
+      <c r="H5" s="125" t="s">
+        <v>613</v>
+      </c>
+      <c r="I5" s="125" t="s">
+        <v>614</v>
+      </c>
+      <c r="J5" s="71"/>
+      <c r="K5" s="79" t="str">
+        <f>'Dashboard financeiro anual'!L4</f>
+        <v>Som e imagem</v>
+      </c>
+      <c r="L5" s="77" t="s">
         <v>595</v>
       </c>
-      <c r="I5" s="87" t="s">
+      <c r="M5" s="77" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="80">
+        <v>1</v>
+      </c>
+      <c r="H6" s="128">
+        <f>SUMIFS(TbRegistrosSaida[Valor],TbRegistrosSaida[Mês previsto],G6,TbRegistrosSaida[Ano Previsto],$D$5,TbRegistrosSaida[Data do Caixa Realizado],"")</f>
+        <v>5159</v>
+      </c>
+      <c r="I6" s="131">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês previsto],G6,TbRegistroEntradas[Ano Previsto],$D$5,TbRegistroEntradas[Data do Caixa Realizado],"")</f>
+        <v>483</v>
+      </c>
+      <c r="J6" s="71"/>
+      <c r="K6" s="81">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Conta Nível 2],$K$5,TbRegistroEntradas[Ano 
+Competência],$M$4,TbRegistroEntradas[Mês 
+Competência],G6)</f>
+        <v>2564</v>
+      </c>
+      <c r="L6" s="81">
+        <f>IF(K6=0,"Não Disp",K6)</f>
+        <v>2564</v>
+      </c>
+      <c r="M6" s="82" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="71">
+        <v>2</v>
+      </c>
+      <c r="H7" s="129">
+        <f>SUMIFS(TbRegistrosSaida[Valor],TbRegistrosSaida[Mês previsto],G7,TbRegistrosSaida[Ano Previsto],$D$5,TbRegistrosSaida[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="126">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês previsto],G7,TbRegistroEntradas[Ano Previsto],$D$5,TbRegistroEntradas[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="71"/>
+      <c r="K7" s="83">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Conta Nível 2],$K$5,TbRegistroEntradas[Ano 
+Competência],$M$4,TbRegistroEntradas[Mês 
+Competência],G7)</f>
+        <v>4732</v>
+      </c>
+      <c r="L7" s="83">
+        <f t="shared" ref="L7:L17" si="0">IF(K7=0,"Não Disp",K7)</f>
+        <v>4732</v>
+      </c>
+      <c r="M7" s="74" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="71"/>
+      <c r="C8" s="73" t="s">
         <v>596</v>
       </c>
-      <c r="J5" s="81"/>
-      <c r="K5" s="89"/>
-      <c r="L5" s="87" t="s">
-        <v>597</v>
-      </c>
-      <c r="M5" s="87" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="81"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
-      <c r="E6" s="81"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="90">
-        <v>1</v>
-      </c>
-      <c r="H6" s="91"/>
-      <c r="I6" s="91"/>
-      <c r="J6" s="81"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="91"/>
-      <c r="M6" s="92" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="81">
-        <v>2</v>
-      </c>
-      <c r="H7" s="93"/>
-      <c r="I7" s="93"/>
-      <c r="J7" s="81"/>
-      <c r="K7" s="93"/>
-      <c r="L7" s="93"/>
-      <c r="M7" s="84" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="81"/>
-      <c r="C8" s="83" t="s">
-        <v>598</v>
-      </c>
-      <c r="D8" s="81"/>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
-      <c r="G8" s="81">
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71">
         <v>3</v>
       </c>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="81"/>
-      <c r="K8" s="93"/>
-      <c r="L8" s="93"/>
-      <c r="M8" s="84" t="s">
+      <c r="H8" s="129">
+        <f>SUMIFS(TbRegistrosSaida[Valor],TbRegistrosSaida[Mês previsto],G8,TbRegistrosSaida[Ano Previsto],$D$5,TbRegistrosSaida[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="126">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês previsto],G8,TbRegistroEntradas[Ano Previsto],$D$5,TbRegistroEntradas[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="71"/>
+      <c r="K8" s="83">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Conta Nível 2],$K$5,TbRegistroEntradas[Ano 
+Competência],$M$4,TbRegistroEntradas[Mês 
+Competência],G8)</f>
+        <v>5489</v>
+      </c>
+      <c r="L8" s="83">
+        <f t="shared" si="0"/>
+        <v>5489</v>
+      </c>
+      <c r="M8" s="74" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="81"/>
-      <c r="C9" s="90" t="s">
+      <c r="B9" s="71"/>
+      <c r="C9" s="80" t="s">
         <v>553</v>
       </c>
-      <c r="D9" s="94">
+      <c r="D9" s="84">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Ano Caixa],"&lt;"&amp;D5,TbRegistroEntradas[Ano Caixa],"&lt;&gt;0")-SUMIFS(TbRegistrosSaida[Valor],TbRegistrosSaida[Ano Caixa],"&lt;"&amp;D5,TbRegistrosSaida[Ano Caixa],"&lt;&gt;0")</f>
         <v>14746</v>
       </c>
-      <c r="E9" s="81"/>
-      <c r="F9" s="81"/>
-      <c r="G9" s="81">
+      <c r="E9" s="106"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="71">
         <v>4</v>
       </c>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="81"/>
-      <c r="K9" s="93"/>
-      <c r="L9" s="93"/>
-      <c r="M9" s="84" t="s">
+      <c r="H9" s="129">
+        <f>SUMIFS(TbRegistrosSaida[Valor],TbRegistrosSaida[Mês previsto],G9,TbRegistrosSaida[Ano Previsto],$D$5,TbRegistrosSaida[Data do Caixa Realizado],"")</f>
+        <v>1753</v>
+      </c>
+      <c r="I9" s="126">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês previsto],G9,TbRegistroEntradas[Ano Previsto],$D$5,TbRegistroEntradas[Data do Caixa Realizado],"")</f>
+        <v>928</v>
+      </c>
+      <c r="J9" s="71"/>
+      <c r="K9" s="83">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Conta Nível 2],$K$5,TbRegistroEntradas[Ano 
+Competência],$M$4,TbRegistroEntradas[Mês 
+Competência],G9)</f>
+        <v>618</v>
+      </c>
+      <c r="L9" s="83">
+        <f t="shared" si="0"/>
+        <v>618</v>
+      </c>
+      <c r="M9" s="74" t="s">
         <v>544</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="81"/>
-      <c r="C10" s="81" t="s">
+      <c r="B10" s="71"/>
+      <c r="C10" s="71" t="s">
         <v>538</v>
       </c>
-      <c r="D10" s="95">
+      <c r="D10" s="85">
         <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Ano Caixa],"="&amp;D5)</f>
         <v>161998</v>
       </c>
-      <c r="E10" s="81"/>
-      <c r="F10" s="81"/>
-      <c r="G10" s="81">
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71">
         <v>5</v>
       </c>
-      <c r="H10" s="93"/>
-      <c r="I10" s="93"/>
-      <c r="J10" s="81"/>
-      <c r="K10" s="93"/>
-      <c r="L10" s="93"/>
-      <c r="M10" s="84" t="s">
+      <c r="H10" s="129">
+        <f>SUMIFS(TbRegistrosSaida[Valor],TbRegistrosSaida[Mês previsto],G10,TbRegistrosSaida[Ano Previsto],$D$5,TbRegistrosSaida[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="126">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês previsto],G10,TbRegistroEntradas[Ano Previsto],$D$5,TbRegistroEntradas[Data do Caixa Realizado],"")</f>
+        <v>2015</v>
+      </c>
+      <c r="J10" s="71"/>
+      <c r="K10" s="83">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Conta Nível 2],$K$5,TbRegistroEntradas[Ano 
+Competência],$M$4,TbRegistroEntradas[Mês 
+Competência],G10)</f>
+        <v>1654</v>
+      </c>
+      <c r="L10" s="83">
+        <f t="shared" si="0"/>
+        <v>1654</v>
+      </c>
+      <c r="M10" s="74" t="s">
         <v>545</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="81"/>
-      <c r="C11" s="81" t="s">
+      <c r="B11" s="71"/>
+      <c r="C11" s="71" t="s">
         <v>539</v>
       </c>
-      <c r="D11" s="95">
+      <c r="D11" s="85">
         <f>SUMIFS(TbRegistrosSaida[Valor],TbRegistrosSaida[Ano Caixa],"="&amp;D5)</f>
         <v>179841</v>
       </c>
-      <c r="E11" s="81"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81">
+      <c r="E11" s="71"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="71">
         <v>6</v>
       </c>
-      <c r="H11" s="93"/>
-      <c r="I11" s="93"/>
-      <c r="J11" s="81"/>
-      <c r="K11" s="93"/>
-      <c r="L11" s="93"/>
-      <c r="M11" s="84" t="s">
+      <c r="H11" s="129">
+        <f>SUMIFS(TbRegistrosSaida[Valor],TbRegistrosSaida[Mês previsto],G11,TbRegistrosSaida[Ano Previsto],$D$5,TbRegistrosSaida[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="126">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês previsto],G11,TbRegistroEntradas[Ano Previsto],$D$5,TbRegistroEntradas[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="71"/>
+      <c r="K11" s="83">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Conta Nível 2],$K$5,TbRegistroEntradas[Ano 
+Competência],$M$4,TbRegistroEntradas[Mês 
+Competência],G11)</f>
+        <v>555</v>
+      </c>
+      <c r="L11" s="83">
+        <f t="shared" si="0"/>
+        <v>555</v>
+      </c>
+      <c r="M11" s="74" t="s">
         <v>546</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="81"/>
-      <c r="C12" s="96" t="s">
-        <v>599</v>
-      </c>
-      <c r="D12" s="97">
+      <c r="B12" s="71"/>
+      <c r="C12" s="86" t="s">
+        <v>597</v>
+      </c>
+      <c r="D12" s="87">
         <f>D9+D10-D11</f>
         <v>-3097</v>
       </c>
-      <c r="E12" s="81"/>
-      <c r="F12" s="81"/>
-      <c r="G12" s="81">
+      <c r="E12" s="71"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="71">
         <v>7</v>
       </c>
-      <c r="H12" s="93"/>
-      <c r="I12" s="93"/>
-      <c r="J12" s="81"/>
-      <c r="K12" s="93"/>
-      <c r="L12" s="93"/>
-      <c r="M12" s="84" t="s">
+      <c r="H12" s="129">
+        <f>SUMIFS(TbRegistrosSaida[Valor],TbRegistrosSaida[Mês previsto],G12,TbRegistrosSaida[Ano Previsto],$D$5,TbRegistrosSaida[Data do Caixa Realizado],"")</f>
+        <v>2338</v>
+      </c>
+      <c r="I12" s="126">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês previsto],G12,TbRegistroEntradas[Ano Previsto],$D$5,TbRegistroEntradas[Data do Caixa Realizado],"")</f>
+        <v>1987</v>
+      </c>
+      <c r="J12" s="71"/>
+      <c r="K12" s="83">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Conta Nível 2],$K$5,TbRegistroEntradas[Ano 
+Competência],$M$4,TbRegistroEntradas[Mês 
+Competência],G12)</f>
+        <v>0</v>
+      </c>
+      <c r="L12" s="83" t="str">
+        <f t="shared" si="0"/>
+        <v>Não Disp</v>
+      </c>
+      <c r="M12" s="74" t="s">
         <v>547</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="81"/>
-      <c r="C13" s="81"/>
-      <c r="D13" s="81"/>
-      <c r="E13" s="124"/>
-      <c r="F13" s="81"/>
-      <c r="G13" s="81">
+      <c r="B13" s="71"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="106"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="71">
         <v>8</v>
       </c>
-      <c r="H13" s="93"/>
-      <c r="I13" s="93"/>
-      <c r="J13" s="81"/>
-      <c r="K13" s="93"/>
-      <c r="L13" s="93"/>
-      <c r="M13" s="84" t="s">
+      <c r="H13" s="129">
+        <f>SUMIFS(TbRegistrosSaida[Valor],TbRegistrosSaida[Mês previsto],G13,TbRegistrosSaida[Ano Previsto],$D$5,TbRegistrosSaida[Data do Caixa Realizado],"")</f>
+        <v>2759</v>
+      </c>
+      <c r="I13" s="126">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês previsto],G13,TbRegistroEntradas[Ano Previsto],$D$5,TbRegistroEntradas[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="71"/>
+      <c r="K13" s="83">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Conta Nível 2],$K$5,TbRegistroEntradas[Ano 
+Competência],$M$4,TbRegistroEntradas[Mês 
+Competência],G13)</f>
+        <v>0</v>
+      </c>
+      <c r="L13" s="83" t="str">
+        <f t="shared" si="0"/>
+        <v>Não Disp</v>
+      </c>
+      <c r="M13" s="74" t="s">
         <v>548</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="81"/>
-      <c r="C14" s="98" t="s">
+      <c r="B14" s="71"/>
+      <c r="C14" s="123" t="s">
+        <v>598</v>
+      </c>
+      <c r="D14" s="123"/>
+      <c r="E14" s="106">
+        <f>SUMIFS(TbRegistrosSaida[Valor],TbRegistrosSaida[Data do Caixa Realizado],"",TbRegistrosSaida[Ano Previsto],D5)</f>
+        <v>12009</v>
+      </c>
+      <c r="F14" s="71"/>
+      <c r="G14" s="71">
+        <v>9</v>
+      </c>
+      <c r="H14" s="129">
+        <f>SUMIFS(TbRegistrosSaida[Valor],TbRegistrosSaida[Mês previsto],G14,TbRegistrosSaida[Ano Previsto],$D$5,TbRegistrosSaida[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="126">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês previsto],G14,TbRegistroEntradas[Ano Previsto],$D$5,TbRegistroEntradas[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="71"/>
+      <c r="K14" s="83">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Conta Nível 2],$K$5,TbRegistroEntradas[Ano 
+Competência],$M$4,TbRegistroEntradas[Mês 
+Competência],G14)</f>
+        <v>0</v>
+      </c>
+      <c r="L14" s="83" t="str">
+        <f t="shared" si="0"/>
+        <v>Não Disp</v>
+      </c>
+      <c r="M14" s="74" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="71"/>
+      <c r="C15" s="124" t="s">
+        <v>599</v>
+      </c>
+      <c r="D15" s="124"/>
+      <c r="E15" s="106">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Data do Caixa Realizado],"",TbRegistroEntradas[Ano Previsto],D5)</f>
+        <v>5413</v>
+      </c>
+      <c r="F15" s="71"/>
+      <c r="G15" s="71">
+        <v>10</v>
+      </c>
+      <c r="H15" s="129">
+        <f>SUMIFS(TbRegistrosSaida[Valor],TbRegistrosSaida[Mês previsto],G15,TbRegistrosSaida[Ano Previsto],$D$5,TbRegistrosSaida[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="126">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês previsto],G15,TbRegistroEntradas[Ano Previsto],$D$5,TbRegistroEntradas[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="71"/>
+      <c r="K15" s="83">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Conta Nível 2],$K$5,TbRegistroEntradas[Ano 
+Competência],$M$4,TbRegistroEntradas[Mês 
+Competência],G15)</f>
+        <v>0</v>
+      </c>
+      <c r="L15" s="83" t="str">
+        <f t="shared" si="0"/>
+        <v>Não Disp</v>
+      </c>
+      <c r="M15" s="74" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="71"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="71"/>
+      <c r="F16" s="71"/>
+      <c r="G16" s="71">
+        <v>11</v>
+      </c>
+      <c r="H16" s="129">
+        <f>SUMIFS(TbRegistrosSaida[Valor],TbRegistrosSaida[Mês previsto],G16,TbRegistrosSaida[Ano Previsto],$D$5,TbRegistrosSaida[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="126">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês previsto],G16,TbRegistroEntradas[Ano Previsto],$D$5,TbRegistroEntradas[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="71"/>
+      <c r="K16" s="83">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Conta Nível 2],$K$5,TbRegistroEntradas[Ano 
+Competência],$M$4,TbRegistroEntradas[Mês 
+Competência],G16)</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="83" t="str">
+        <f t="shared" si="0"/>
+        <v>Não Disp</v>
+      </c>
+      <c r="M16" s="74" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B17" s="71"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="71"/>
+      <c r="G17" s="86">
+        <v>12</v>
+      </c>
+      <c r="H17" s="130">
+        <f>SUMIFS(TbRegistrosSaida[Valor],TbRegistrosSaida[Mês previsto],G17,TbRegistrosSaida[Ano Previsto],$D$5,TbRegistrosSaida[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="127">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Mês previsto],G17,TbRegistroEntradas[Ano Previsto],$D$5,TbRegistroEntradas[Data do Caixa Realizado],"")</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="71"/>
+      <c r="K17" s="88">
+        <f>SUMIFS(TbRegistroEntradas[Valor],TbRegistroEntradas[Conta Nível 2],$K$5,TbRegistroEntradas[Ano 
+Competência],$M$4,TbRegistroEntradas[Mês 
+Competência],G17)</f>
+        <v>0</v>
+      </c>
+      <c r="L17" s="88" t="str">
+        <f t="shared" si="0"/>
+        <v>Não Disp</v>
+      </c>
+      <c r="M17" s="89" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B18" s="71"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="71"/>
+      <c r="K18" s="71"/>
+      <c r="L18" s="71"/>
+      <c r="M18" s="71"/>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B19" s="71"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="71"/>
+      <c r="J19" s="71"/>
+      <c r="K19" s="71"/>
+      <c r="L19" s="71"/>
+      <c r="M19" s="71"/>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" s="71"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="90"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="71"/>
+      <c r="J20" s="71"/>
+      <c r="K20" s="71"/>
+      <c r="L20" s="71"/>
+      <c r="M20" s="71"/>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" s="71"/>
+      <c r="C21" s="73" t="s">
         <v>600</v>
       </c>
-      <c r="D14" s="98"/>
-      <c r="E14" s="124"/>
-      <c r="F14" s="81"/>
-      <c r="G14" s="81">
+      <c r="D21" s="71"/>
+      <c r="E21" s="78" t="s">
+        <v>603</v>
+      </c>
+      <c r="F21" s="78" t="s">
+        <v>581</v>
+      </c>
+      <c r="G21" s="71"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="71"/>
+      <c r="J21" s="71"/>
+      <c r="K21" s="71"/>
+      <c r="L21" s="71"/>
+      <c r="M21" s="71"/>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="71"/>
+      <c r="C22" s="77" t="s">
+        <v>601</v>
+      </c>
+      <c r="D22" s="78" t="s">
+        <v>602</v>
+      </c>
+      <c r="E22" s="92"/>
+      <c r="F22" s="92"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="71"/>
+      <c r="J22" s="71"/>
+      <c r="K22" s="71"/>
+      <c r="L22" s="71"/>
+      <c r="M22" s="71"/>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="71"/>
+      <c r="C23" s="91"/>
+      <c r="D23" s="92"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="71"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="71"/>
+      <c r="J23" s="71"/>
+      <c r="K23" s="71"/>
+      <c r="L23" s="71"/>
+      <c r="M23" s="71"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B24" s="71"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="71"/>
+      <c r="L24" s="71"/>
+      <c r="M24" s="71"/>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" s="71"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="73" t="s">
+        <v>605</v>
+      </c>
+      <c r="I25" s="71"/>
+      <c r="J25" s="71"/>
+      <c r="K25" s="71"/>
+      <c r="L25" s="71"/>
+      <c r="M25" s="71"/>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B26" s="71"/>
+      <c r="C26" s="73" t="s">
+        <v>604</v>
+      </c>
+      <c r="D26" s="71"/>
+      <c r="E26" s="78" t="s">
+        <v>607</v>
+      </c>
+      <c r="F26" s="78" t="s">
+        <v>608</v>
+      </c>
+      <c r="G26" s="71"/>
+      <c r="H26" s="77" t="s">
+        <v>601</v>
+      </c>
+      <c r="I26" s="78" t="s">
+        <v>606</v>
+      </c>
+      <c r="J26" s="78" t="s">
+        <v>607</v>
+      </c>
+      <c r="K26" s="78" t="s">
+        <v>608</v>
+      </c>
+      <c r="L26" s="71"/>
+      <c r="M26" s="71"/>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="71"/>
+      <c r="C27" s="77" t="s">
+        <v>601</v>
+      </c>
+      <c r="D27" s="78" t="s">
+        <v>606</v>
+      </c>
+      <c r="E27" s="93"/>
+      <c r="F27" s="93"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="91"/>
+      <c r="I27" s="93"/>
+      <c r="J27" s="93"/>
+      <c r="K27" s="93"/>
+      <c r="L27" s="71"/>
+      <c r="M27" s="71"/>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="71"/>
+      <c r="C28" s="91"/>
+      <c r="D28" s="93"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="71"/>
+      <c r="K28" s="71"/>
+      <c r="L28" s="71"/>
+      <c r="M28" s="71"/>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="71"/>
+      <c r="C29" s="71"/>
+      <c r="D29" s="71"/>
+      <c r="E29" s="71"/>
+      <c r="F29" s="71"/>
+      <c r="G29" s="71"/>
+      <c r="H29" s="71"/>
+      <c r="I29" s="71"/>
+      <c r="J29" s="71"/>
+      <c r="K29" s="71"/>
+      <c r="L29" s="71"/>
+      <c r="M29" s="71"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="71"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="71"/>
+      <c r="G30" s="71"/>
+      <c r="H30" s="73" t="s">
+        <v>610</v>
+      </c>
+      <c r="I30" s="94"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="71"/>
+      <c r="L30" s="71"/>
+      <c r="M30" s="71"/>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="71"/>
+      <c r="C31" s="73" t="s">
+        <v>609</v>
+      </c>
+      <c r="D31" s="71"/>
+      <c r="E31" s="82" t="s">
+        <v>539</v>
+      </c>
+      <c r="F31" s="82" t="s">
+        <v>612</v>
+      </c>
+      <c r="G31" s="71"/>
+      <c r="H31" s="77" t="s">
+        <v>594</v>
+      </c>
+      <c r="I31" s="96"/>
+      <c r="J31" s="71"/>
+      <c r="K31" s="71"/>
+      <c r="L31" s="71"/>
+      <c r="M31" s="71"/>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="71"/>
+      <c r="C32" s="95" t="s">
+        <v>611</v>
+      </c>
+      <c r="D32" s="82" t="s">
+        <v>538</v>
+      </c>
+      <c r="E32" s="98"/>
+      <c r="F32" s="99"/>
+      <c r="G32" s="71"/>
+      <c r="H32" s="71">
+        <v>1</v>
+      </c>
+      <c r="I32" s="83"/>
+      <c r="J32" s="71"/>
+      <c r="K32" s="71"/>
+      <c r="L32" s="71"/>
+      <c r="M32" s="71"/>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B33" s="71"/>
+      <c r="C33" s="97"/>
+      <c r="D33" s="98"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="71">
+        <v>2</v>
+      </c>
+      <c r="I33" s="83"/>
+      <c r="J33" s="71"/>
+      <c r="K33" s="71"/>
+      <c r="L33" s="71"/>
+      <c r="M33" s="71"/>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B34" s="71"/>
+      <c r="C34" s="71"/>
+      <c r="D34" s="71"/>
+      <c r="E34" s="71"/>
+      <c r="F34" s="71"/>
+      <c r="G34" s="71"/>
+      <c r="H34" s="71">
+        <v>3</v>
+      </c>
+      <c r="I34" s="83"/>
+      <c r="J34" s="71"/>
+      <c r="K34" s="71"/>
+      <c r="L34" s="71"/>
+      <c r="M34" s="71"/>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B35" s="71"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="71"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="71"/>
+      <c r="H35" s="71">
+        <v>4</v>
+      </c>
+      <c r="I35" s="83"/>
+      <c r="J35" s="71"/>
+      <c r="K35" s="71"/>
+      <c r="L35" s="71"/>
+      <c r="M35" s="71"/>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" s="71"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="71"/>
+      <c r="E36" s="71"/>
+      <c r="F36" s="71"/>
+      <c r="G36" s="71"/>
+      <c r="H36" s="71">
+        <v>5</v>
+      </c>
+      <c r="I36" s="83"/>
+      <c r="J36" s="71"/>
+      <c r="K36" s="71"/>
+      <c r="L36" s="71"/>
+      <c r="M36" s="71"/>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B37" s="71"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="71"/>
+      <c r="E37" s="71"/>
+      <c r="F37" s="71"/>
+      <c r="G37" s="71"/>
+      <c r="H37" s="71">
+        <v>6</v>
+      </c>
+      <c r="I37" s="83"/>
+      <c r="J37" s="71"/>
+      <c r="K37" s="71"/>
+      <c r="L37" s="71"/>
+      <c r="M37" s="71"/>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B38" s="71"/>
+      <c r="C38" s="71"/>
+      <c r="D38" s="71"/>
+      <c r="E38" s="71"/>
+      <c r="F38" s="71"/>
+      <c r="G38" s="71"/>
+      <c r="H38" s="71">
+        <v>7</v>
+      </c>
+      <c r="I38" s="83"/>
+      <c r="J38" s="71"/>
+      <c r="K38" s="71"/>
+      <c r="L38" s="71"/>
+      <c r="M38" s="71"/>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B39" s="71"/>
+      <c r="C39" s="71"/>
+      <c r="D39" s="71"/>
+      <c r="E39" s="71"/>
+      <c r="F39" s="71"/>
+      <c r="G39" s="71"/>
+      <c r="H39" s="71">
+        <v>8</v>
+      </c>
+      <c r="I39" s="83"/>
+      <c r="J39" s="71"/>
+      <c r="K39" s="71"/>
+      <c r="L39" s="71"/>
+      <c r="M39" s="71"/>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B40" s="71"/>
+      <c r="C40" s="71"/>
+      <c r="D40" s="71"/>
+      <c r="E40" s="71"/>
+      <c r="F40" s="71"/>
+      <c r="G40" s="71"/>
+      <c r="H40" s="71">
         <v>9</v>
       </c>
-      <c r="H14" s="93"/>
-      <c r="I14" s="93"/>
-      <c r="J14" s="81"/>
-      <c r="K14" s="93"/>
-      <c r="L14" s="93"/>
-      <c r="M14" s="84" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="81"/>
-      <c r="C15" s="99" t="s">
-        <v>601</v>
-      </c>
-      <c r="D15" s="99"/>
-      <c r="E15" s="81"/>
-      <c r="F15" s="81"/>
-      <c r="G15" s="81">
+      <c r="I40" s="83"/>
+      <c r="J40" s="71"/>
+      <c r="K40" s="71"/>
+      <c r="L40" s="71"/>
+      <c r="M40" s="71"/>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B41" s="71"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="71"/>
+      <c r="E41" s="71"/>
+      <c r="F41" s="71"/>
+      <c r="G41" s="71"/>
+      <c r="H41" s="71">
         <v>10</v>
       </c>
-      <c r="H15" s="93"/>
-      <c r="I15" s="93"/>
-      <c r="J15" s="81"/>
-      <c r="K15" s="93"/>
-      <c r="L15" s="93"/>
-      <c r="M15" s="84" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="81"/>
-      <c r="C16" s="81"/>
-      <c r="D16" s="81"/>
-      <c r="E16" s="81"/>
-      <c r="F16" s="81"/>
-      <c r="G16" s="81">
+      <c r="I41" s="83"/>
+      <c r="J41" s="71"/>
+      <c r="K41" s="71"/>
+      <c r="L41" s="71"/>
+      <c r="M41" s="71"/>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B42" s="71"/>
+      <c r="C42" s="71"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="71"/>
+      <c r="F42" s="71"/>
+      <c r="G42" s="71"/>
+      <c r="H42" s="71">
         <v>11</v>
       </c>
-      <c r="H16" s="93"/>
-      <c r="I16" s="93"/>
-      <c r="J16" s="81"/>
-      <c r="K16" s="93"/>
-      <c r="L16" s="93"/>
-      <c r="M16" s="84" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="81"/>
-      <c r="C17" s="81"/>
-      <c r="D17" s="81"/>
-      <c r="E17" s="81"/>
-      <c r="F17" s="81"/>
-      <c r="G17" s="96">
+      <c r="I42" s="83"/>
+      <c r="J42" s="71"/>
+      <c r="K42" s="71"/>
+      <c r="L42" s="71"/>
+      <c r="M42" s="71"/>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B43" s="71"/>
+      <c r="C43" s="71"/>
+      <c r="D43" s="71"/>
+      <c r="E43" s="71"/>
+      <c r="F43" s="71"/>
+      <c r="G43" s="71"/>
+      <c r="H43" s="86">
         <v>12</v>
       </c>
-      <c r="H17" s="100"/>
-      <c r="I17" s="100"/>
-      <c r="J17" s="81"/>
-      <c r="K17" s="100"/>
-      <c r="L17" s="100"/>
-      <c r="M17" s="101" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="81"/>
-      <c r="C18" s="81"/>
-      <c r="D18" s="81"/>
-      <c r="E18" s="81"/>
-      <c r="F18" s="81"/>
-      <c r="G18" s="81"/>
-      <c r="H18" s="81"/>
-      <c r="I18" s="81"/>
-      <c r="J18" s="81"/>
-      <c r="K18" s="81"/>
-      <c r="L18" s="81"/>
-      <c r="M18" s="81"/>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="81"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="81"/>
-      <c r="E19" s="81"/>
-      <c r="F19" s="81"/>
-      <c r="G19" s="81"/>
-      <c r="H19" s="81"/>
-      <c r="I19" s="81"/>
-      <c r="J19" s="81"/>
-      <c r="K19" s="81"/>
-      <c r="L19" s="81"/>
-      <c r="M19" s="81"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="81"/>
-      <c r="C20" s="81"/>
-      <c r="D20" s="81"/>
-      <c r="E20" s="81"/>
-      <c r="F20" s="102"/>
-      <c r="G20" s="81"/>
-      <c r="H20" s="81"/>
-      <c r="I20" s="81"/>
-      <c r="J20" s="81"/>
-      <c r="K20" s="81"/>
-      <c r="L20" s="81"/>
-      <c r="M20" s="81"/>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="81"/>
-      <c r="C21" s="83" t="s">
-        <v>602</v>
-      </c>
-      <c r="D21" s="81"/>
-      <c r="E21" s="88" t="s">
-        <v>605</v>
-      </c>
-      <c r="F21" s="88" t="s">
+      <c r="I43" s="88"/>
+      <c r="J43" s="71"/>
+      <c r="K43" s="71"/>
+      <c r="L43" s="71"/>
+      <c r="M43" s="71"/>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B44" s="71"/>
+      <c r="C44" s="71"/>
+      <c r="D44" s="71"/>
+      <c r="E44" s="71"/>
+      <c r="F44" s="71"/>
+      <c r="G44" s="71"/>
+      <c r="H44" s="77" t="s">
         <v>581</v>
       </c>
-      <c r="G21" s="81"/>
-      <c r="H21" s="81"/>
-      <c r="I21" s="81"/>
-      <c r="J21" s="81"/>
-      <c r="K21" s="81"/>
-      <c r="L21" s="81"/>
-      <c r="M21" s="81"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="81"/>
-      <c r="C22" s="87" t="s">
-        <v>603</v>
-      </c>
-      <c r="D22" s="88" t="s">
-        <v>604</v>
-      </c>
-      <c r="E22" s="104"/>
-      <c r="F22" s="104"/>
-      <c r="G22" s="81"/>
-      <c r="H22" s="81"/>
-      <c r="I22" s="81"/>
-      <c r="J22" s="81"/>
-      <c r="K22" s="81"/>
-      <c r="L22" s="81"/>
-      <c r="M22" s="81"/>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="81"/>
-      <c r="C23" s="103"/>
-      <c r="D23" s="104"/>
-      <c r="E23" s="81"/>
-      <c r="F23" s="81"/>
-      <c r="G23" s="81"/>
-      <c r="H23" s="81"/>
-      <c r="I23" s="81"/>
-      <c r="J23" s="81"/>
-      <c r="K23" s="81"/>
-      <c r="L23" s="81"/>
-      <c r="M23" s="81"/>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="81"/>
-      <c r="C24" s="81"/>
-      <c r="D24" s="81"/>
-      <c r="E24" s="81"/>
-      <c r="F24" s="81"/>
-      <c r="G24" s="81"/>
-      <c r="H24" s="81"/>
-      <c r="I24" s="81"/>
-      <c r="J24" s="81"/>
-      <c r="K24" s="81"/>
-      <c r="L24" s="81"/>
-      <c r="M24" s="81"/>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="81"/>
-      <c r="C25" s="81"/>
-      <c r="D25" s="81"/>
-      <c r="E25" s="81"/>
-      <c r="F25" s="81"/>
-      <c r="G25" s="81"/>
-      <c r="H25" s="83" t="s">
-        <v>607</v>
-      </c>
-      <c r="I25" s="81"/>
-      <c r="J25" s="81"/>
-      <c r="K25" s="81"/>
-      <c r="L25" s="81"/>
-      <c r="M25" s="81"/>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="81"/>
-      <c r="C26" s="83" t="s">
-        <v>606</v>
-      </c>
-      <c r="D26" s="81"/>
-      <c r="E26" s="88" t="s">
-        <v>609</v>
-      </c>
-      <c r="F26" s="88" t="s">
-        <v>610</v>
-      </c>
-      <c r="G26" s="81"/>
-      <c r="H26" s="87" t="s">
-        <v>603</v>
-      </c>
-      <c r="I26" s="88" t="s">
-        <v>608</v>
-      </c>
-      <c r="J26" s="88" t="s">
-        <v>609</v>
-      </c>
-      <c r="K26" s="88" t="s">
-        <v>610</v>
-      </c>
-      <c r="L26" s="81"/>
-      <c r="M26" s="81"/>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="81"/>
-      <c r="C27" s="87" t="s">
-        <v>603</v>
-      </c>
-      <c r="D27" s="88" t="s">
-        <v>608</v>
-      </c>
-      <c r="E27" s="105"/>
-      <c r="F27" s="105"/>
-      <c r="G27" s="81"/>
-      <c r="H27" s="103"/>
-      <c r="I27" s="105"/>
-      <c r="J27" s="105"/>
-      <c r="K27" s="105"/>
-      <c r="L27" s="81"/>
-      <c r="M27" s="81"/>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="81"/>
-      <c r="C28" s="103"/>
-      <c r="D28" s="105"/>
-      <c r="E28" s="81"/>
-      <c r="F28" s="81"/>
-      <c r="G28" s="81"/>
-      <c r="H28" s="81"/>
-      <c r="I28" s="81"/>
-      <c r="J28" s="81"/>
-      <c r="K28" s="81"/>
-      <c r="L28" s="81"/>
-      <c r="M28" s="81"/>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="81"/>
-      <c r="C29" s="81"/>
-      <c r="D29" s="81"/>
-      <c r="E29" s="81"/>
-      <c r="F29" s="81"/>
-      <c r="G29" s="81"/>
-      <c r="H29" s="81"/>
-      <c r="I29" s="81"/>
-      <c r="J29" s="81"/>
-      <c r="K29" s="81"/>
-      <c r="L29" s="81"/>
-      <c r="M29" s="81"/>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B30" s="81"/>
-      <c r="C30" s="81"/>
-      <c r="D30" s="81"/>
-      <c r="E30" s="81"/>
-      <c r="F30" s="81"/>
-      <c r="G30" s="81"/>
-      <c r="H30" s="83" t="s">
-        <v>612</v>
-      </c>
-      <c r="I30" s="106"/>
-      <c r="J30" s="81"/>
-      <c r="K30" s="81"/>
-      <c r="L30" s="81"/>
-      <c r="M30" s="81"/>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="81"/>
-      <c r="C31" s="83" t="s">
-        <v>611</v>
-      </c>
-      <c r="D31" s="81"/>
-      <c r="E31" s="92" t="s">
-        <v>539</v>
-      </c>
-      <c r="F31" s="92" t="s">
-        <v>614</v>
-      </c>
-      <c r="G31" s="81"/>
-      <c r="H31" s="87" t="s">
-        <v>594</v>
-      </c>
-      <c r="I31" s="108"/>
-      <c r="J31" s="81"/>
-      <c r="K31" s="81"/>
-      <c r="L31" s="81"/>
-      <c r="M31" s="81"/>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="81"/>
-      <c r="C32" s="107" t="s">
-        <v>613</v>
-      </c>
-      <c r="D32" s="92" t="s">
-        <v>538</v>
-      </c>
-      <c r="E32" s="110"/>
-      <c r="F32" s="111"/>
-      <c r="G32" s="81"/>
-      <c r="H32" s="81">
-        <v>1</v>
-      </c>
-      <c r="I32" s="93"/>
-      <c r="J32" s="81"/>
-      <c r="K32" s="81"/>
-      <c r="L32" s="81"/>
-      <c r="M32" s="81"/>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B33" s="81"/>
-      <c r="C33" s="109"/>
-      <c r="D33" s="110"/>
-      <c r="E33" s="81"/>
-      <c r="F33" s="81"/>
-      <c r="G33" s="81"/>
-      <c r="H33" s="81">
-        <v>2</v>
-      </c>
-      <c r="I33" s="93"/>
-      <c r="J33" s="81"/>
-      <c r="K33" s="81"/>
-      <c r="L33" s="81"/>
-      <c r="M33" s="81"/>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B34" s="81"/>
-      <c r="C34" s="81"/>
-      <c r="D34" s="81"/>
-      <c r="E34" s="81"/>
-      <c r="F34" s="81"/>
-      <c r="G34" s="81"/>
-      <c r="H34" s="81">
-        <v>3</v>
-      </c>
-      <c r="I34" s="93"/>
-      <c r="J34" s="81"/>
-      <c r="K34" s="81"/>
-      <c r="L34" s="81"/>
-      <c r="M34" s="81"/>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="81"/>
-      <c r="C35" s="81"/>
-      <c r="D35" s="81"/>
-      <c r="E35" s="81"/>
-      <c r="F35" s="81"/>
-      <c r="G35" s="81"/>
-      <c r="H35" s="81">
-        <v>4</v>
-      </c>
-      <c r="I35" s="93"/>
-      <c r="J35" s="81"/>
-      <c r="K35" s="81"/>
-      <c r="L35" s="81"/>
-      <c r="M35" s="81"/>
-    </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B36" s="81"/>
-      <c r="C36" s="81"/>
-      <c r="D36" s="81"/>
-      <c r="E36" s="81"/>
-      <c r="F36" s="81"/>
-      <c r="G36" s="81"/>
-      <c r="H36" s="81">
-        <v>5</v>
-      </c>
-      <c r="I36" s="93"/>
-      <c r="J36" s="81"/>
-      <c r="K36" s="81"/>
-      <c r="L36" s="81"/>
-      <c r="M36" s="81"/>
-    </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B37" s="81"/>
-      <c r="C37" s="81"/>
-      <c r="D37" s="81"/>
-      <c r="E37" s="81"/>
-      <c r="F37" s="81"/>
-      <c r="G37" s="81"/>
-      <c r="H37" s="81">
-        <v>6</v>
-      </c>
-      <c r="I37" s="93"/>
-      <c r="J37" s="81"/>
-      <c r="K37" s="81"/>
-      <c r="L37" s="81"/>
-      <c r="M37" s="81"/>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B38" s="81"/>
-      <c r="C38" s="81"/>
-      <c r="D38" s="81"/>
-      <c r="E38" s="81"/>
-      <c r="F38" s="81"/>
-      <c r="G38" s="81"/>
-      <c r="H38" s="81">
-        <v>7</v>
-      </c>
-      <c r="I38" s="93"/>
-      <c r="J38" s="81"/>
-      <c r="K38" s="81"/>
-      <c r="L38" s="81"/>
-      <c r="M38" s="81"/>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B39" s="81"/>
-      <c r="C39" s="81"/>
-      <c r="D39" s="81"/>
-      <c r="E39" s="81"/>
-      <c r="F39" s="81"/>
-      <c r="G39" s="81"/>
-      <c r="H39" s="81">
-        <v>8</v>
-      </c>
-      <c r="I39" s="93"/>
-      <c r="J39" s="81"/>
-      <c r="K39" s="81"/>
-      <c r="L39" s="81"/>
-      <c r="M39" s="81"/>
-    </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B40" s="81"/>
-      <c r="C40" s="81"/>
-      <c r="D40" s="81"/>
-      <c r="E40" s="81"/>
-      <c r="F40" s="81"/>
-      <c r="G40" s="81"/>
-      <c r="H40" s="81">
-        <v>9</v>
-      </c>
-      <c r="I40" s="93"/>
-      <c r="J40" s="81"/>
-      <c r="K40" s="81"/>
-      <c r="L40" s="81"/>
-      <c r="M40" s="81"/>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B41" s="81"/>
-      <c r="C41" s="81"/>
-      <c r="D41" s="81"/>
-      <c r="E41" s="81"/>
-      <c r="F41" s="81"/>
-      <c r="G41" s="81"/>
-      <c r="H41" s="81">
-        <v>10</v>
-      </c>
-      <c r="I41" s="93"/>
-      <c r="J41" s="81"/>
-      <c r="K41" s="81"/>
-      <c r="L41" s="81"/>
-      <c r="M41" s="81"/>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B42" s="81"/>
-      <c r="C42" s="81"/>
-      <c r="D42" s="81"/>
-      <c r="E42" s="81"/>
-      <c r="F42" s="81"/>
-      <c r="G42" s="81"/>
-      <c r="H42" s="81">
-        <v>11</v>
-      </c>
-      <c r="I42" s="93"/>
-      <c r="J42" s="81"/>
-      <c r="K42" s="81"/>
-      <c r="L42" s="81"/>
-      <c r="M42" s="81"/>
-    </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B43" s="81"/>
-      <c r="C43" s="81"/>
-      <c r="D43" s="81"/>
-      <c r="E43" s="81"/>
-      <c r="F43" s="81"/>
-      <c r="G43" s="81"/>
-      <c r="H43" s="96">
-        <v>12</v>
-      </c>
-      <c r="I43" s="100"/>
-      <c r="J43" s="81"/>
-      <c r="K43" s="81"/>
-      <c r="L43" s="81"/>
-      <c r="M43" s="81"/>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B44" s="81"/>
-      <c r="C44" s="81"/>
-      <c r="D44" s="81"/>
-      <c r="E44" s="81"/>
-      <c r="F44" s="81"/>
-      <c r="G44" s="81"/>
-      <c r="H44" s="87" t="s">
-        <v>581</v>
-      </c>
-      <c r="I44" s="112"/>
-      <c r="J44" s="81"/>
-      <c r="K44" s="81"/>
-      <c r="L44" s="81"/>
-      <c r="M44" s="81"/>
+      <c r="I44" s="100"/>
+      <c r="J44" s="71"/>
+      <c r="K44" s="71"/>
+      <c r="L44" s="71"/>
+      <c r="M44" s="71"/>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C45" s="81"/>
-      <c r="D45" s="81"/>
+      <c r="C45" s="71"/>
+      <c r="D45" s="71"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+  </mergeCells>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20344,9 +21369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -20856,7 +21879,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20975,7 +21998,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21020,10 +22043,10 @@
       <c r="N2" s="6"/>
     </row>
     <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="107" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="63"/>
+      <c r="C3" s="108"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -21318,10 +22341,10 @@
       <c r="N2" s="6"/>
     </row>
     <row r="3" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="109" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="65"/>
+      <c r="C3" s="110"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -21467,9 +22490,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O236"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H151" sqref="H151:H236"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6:O236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44351,11 +45374,11 @@
       </c>
     </row>
     <row r="7" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="111" t="s">
         <v>536</v>
       </c>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
+      <c r="C7" s="111"/>
+      <c r="D7" s="111"/>
     </row>
     <row r="8" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="30" t="s">
@@ -44613,12 +45636,12 @@
     <row r="13" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="67" t="s">
+      <c r="B15" s="112" t="s">
         <v>554</v>
       </c>
-      <c r="C15" s="67"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="67"/>
+      <c r="C15" s="112"/>
+      <c r="D15" s="112"/>
+      <c r="E15" s="112"/>
     </row>
     <row r="16" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="30" t="s">
@@ -44928,12 +45951,12 @@
     <row r="21" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="68" t="s">
+      <c r="B23" s="113" t="s">
         <v>555</v>
       </c>
-      <c r="C23" s="68"/>
-      <c r="D23" s="68"/>
-      <c r="E23" s="68"/>
+      <c r="C23" s="113"/>
+      <c r="D23" s="113"/>
+      <c r="E23" s="113"/>
     </row>
     <row r="24" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="30" t="s">

</xml_diff>